<commit_message>
Added dependency ids to DRA tests.
</commit_message>
<xml_diff>
--- a/src/test/test-data/DRAContainerTestData.xlsx
+++ b/src/test/test-data/DRAContainerTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="104">
   <si>
     <t>API</t>
   </si>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1267,7 +1267,9 @@
       <c r="H16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="J16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1393,7 +1395,9 @@
         <v>55</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="J20" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Fixed IPA, DRA container failed tests
</commit_message>
<xml_diff>
--- a/src/test/test-data/DRAContainerTestData.xlsx
+++ b/src/test/test-data/DRAContainerTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="103">
   <si>
     <t>API</t>
   </si>
@@ -82,9 +87,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>status=200||public_count=0||private_count=0||total_count=0</t>
-  </si>
-  <si>
     <t>{ "ispublic": true }</t>
   </si>
   <si>
@@ -103,9 +105,6 @@
     <t>X-1P-User=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||public_count=1||private_count=1||total_count=2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that saved work counts are shown as zero when user doesn't have any saved works using container API. </t>
   </si>
   <si>
@@ -124,9 +123,6 @@
     <t>{"name":"Second DRA Container by Project Neon1","type":"dra_ss","ispublic":false, "desc": "Second SSE - DRA Container created by postman"}</t>
   </si>
   <si>
-    <t>status=200||type=dra_ss||name=Second DRA Container by Project Neon1||desc=Second SSE - DRA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>Verify that user is able to update DRA container name using container API</t>
   </si>
   <si>
@@ -196,15 +192,6 @@
     <t>Verify that deleted DRA container can't be deleted  and check the error status using container API</t>
   </si>
   <si>
-    <t>Verify that last viewed time can be updated for a particular saved search under a particular DRA container using container API</t>
-  </si>
-  <si>
-    <t>{"lastViewed":1481190745991,"type":"dra_td_sse"}</t>
-  </si>
-  <si>
-    <t>status=200||type=dra_ss||name=First DRA Container by Project Neon1||desc=First SSE - DRA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>{"items":[{"attributes":{"searchTerm":"Cancer, prostate neuroendocrine","searchUrl":"{\"searchId\":\"96954ca8-e7be-4fac-8273-ebd3d1ca6ace\",\"hits\":12,\"took\":36,\"terms\":{\"boolop\":\"OR\",\"searchTerms\":{\"conditions\":[\"Cancer, prostate neuroendocrine\"]}},\"active\":true,\"inputs\":{\"method\":\"POST\",\"path\":\"search/visualization/96954ca8-e7be-4fac-8273-ebd3d1ca6ace\",\"type\":\"bubble\",\"offset\":null,\"size\":null,\"sizeBy\":\"drugCount\",\"colorBy\":\"highestPhase-HighestPhase\",\"colorType\":\"HighestPhase\",\"clusterBy\":\"targetFamily\",\"publish\":true}}","name":"simple search: Cancer, prostate-neuroendocrine","description":"Simple cancer search - DRA from Postman"},"type":"dra_td_sse","id":"211"}]}</t>
   </si>
   <si>
@@ -256,9 +243,6 @@
     <t>/container/(OPQA-4615_id)</t>
   </si>
   <si>
-    <t>status=200||public_count=1||private_count=1||total_count=2||private[0].id=(OPQA-4614_id)||private[0].contents.dra_td_sse=2||private[0].contents.total=2||public[0].id=(OPQA-4615_id)||public[0].contents.dra_td_sse=0||public[0].contents.total=0</t>
-  </si>
-  <si>
     <t>OPQA-4616</t>
   </si>
   <si>
@@ -304,9 +288,6 @@
     <t>OPQA-4627</t>
   </si>
   <si>
-    <t>OPQA-4628</t>
-  </si>
-  <si>
     <t>OPQA-4629</t>
   </si>
   <si>
@@ -326,13 +307,35 @@
   </si>
   <si>
     <t>OPQA-4634</t>
+  </si>
+  <si>
+    <t>status=200||type=dra_ss||name=First DRA Container by Project Neon1||desc=First SSE - DRA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=true</t>
+  </si>
+  <si>
+    <t>status=200||type=dra_ss||name=Second DRA Container by Project Neon1||desc=Second SSE - DRA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=true</t>
+  </si>
+  <si>
+    <t>status=200||public_count=0||private_count=1||total_count=1</t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=2||total_count=3</t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=2||total_count=3||private[0].id=(OPQA-4614_id)||private[0].contents.dra_td_sse=2||private[0].contents.total=2||public[0].id=(OPQA-4615_id)||public[0].contents.dra_td_sse=0||public[0].contents.total=0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +451,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -494,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,9 +537,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -560,6 +572,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,30 +748,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="31.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="52.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="31.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -796,12 +809,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>19</v>
@@ -816,22 +829,24 @@
         <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2"/>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2"/>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>19</v>
@@ -847,23 +862,25 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3"/>
       <c r="J3" s="2" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>19</v>
@@ -879,29 +896,31 @@
       </c>
       <c r="G4"/>
       <c r="H4" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4"/>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -911,29 +930,31 @@
       </c>
       <c r="G5"/>
       <c r="H5" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -943,29 +964,31 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -975,91 +998,97 @@
       </c>
       <c r="G7"/>
       <c r="H7" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="L7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="30">
+      <c r="L8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H9"/>
       <c r="I9" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="30">
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
@@ -1070,26 +1099,28 @@
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K10"/>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="L10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -1099,23 +1130,25 @@
       </c>
       <c r="G11"/>
       <c r="H11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="47.25">
+      <c r="L11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>19</v>
@@ -1130,30 +1163,32 @@
         <v>17</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="255">
+      <c r="L12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -1162,66 +1197,70 @@
         <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="255">
+      <c r="L13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="K14" s="2"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="360">
+      <c r="L14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
@@ -1230,32 +1269,34 @@
         <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="255">
-      <c r="A16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1265,61 +1306,65 @@
       </c>
       <c r="G16"/>
       <c r="H16" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" ht="60">
-      <c r="A17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17"/>
-      <c r="H17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="135">
-      <c r="A18" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
@@ -1328,62 +1373,66 @@
         <v>17</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="45">
+      <c r="L18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>45</v>
+      <c r="G19" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="45">
+      <c r="L19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>18</v>
@@ -1391,25 +1440,25 @@
       <c r="F20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" ht="30">
-      <c r="A21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>19</v>
@@ -1421,48 +1470,56 @@
         <v>18</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G21"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" ht="45">
+      <c r="L21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>28</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G22"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" ht="30">
+        <v>13</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>56</v>
@@ -1471,47 +1528,25 @@
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="G23"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="45">
-      <c r="A24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>